<commit_message>
Update 2018 Meskel Promises.xlsx data
</commit_message>
<xml_diff>
--- a/2018 Meskel Promises.xlsx
+++ b/2018 Meskel Promises.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\OneDrive\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\OneDrive\Desktop\meskel_app\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13140" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="55">
   <si>
     <t>Name</t>
   </si>
@@ -35,28 +35,160 @@
     <t>Promises</t>
   </si>
   <si>
-    <t>2 sheep and 1 bottle of honey</t>
-  </si>
-  <si>
-    <t>Hana Tesfaye</t>
-  </si>
-  <si>
-    <t>5 loaves of bread</t>
-  </si>
-  <si>
-    <t>Dawit Mekonnen</t>
-  </si>
-  <si>
-    <t>1 drum of tella (local beer)</t>
-  </si>
-  <si>
-    <t>Meskerem Lema</t>
-  </si>
-  <si>
-    <t>200 birr contribution</t>
-  </si>
-  <si>
     <t>Biruk Mulu</t>
+  </si>
+  <si>
+    <t>3000 ETB</t>
+  </si>
+  <si>
+    <t>Fantanesh Muluneh</t>
+  </si>
+  <si>
+    <t>Bereket Mulu</t>
+  </si>
+  <si>
+    <t>20 Injera and 1 loaves of bread</t>
+  </si>
+  <si>
+    <t>Dagmawi Awoke</t>
+  </si>
+  <si>
+    <t>Mulu Alemu</t>
+  </si>
+  <si>
+    <t>600 ETB</t>
+  </si>
+  <si>
+    <t>Binyam Mulu</t>
+  </si>
+  <si>
+    <t>1 Sheep</t>
+  </si>
+  <si>
+    <t>Awoke Mulu</t>
+  </si>
+  <si>
+    <t>4000 ETB</t>
+  </si>
+  <si>
+    <t>Felekech</t>
+  </si>
+  <si>
+    <t>1 Taba Kitfo and 4 Kocho</t>
+  </si>
+  <si>
+    <t>Yezena Hibist</t>
+  </si>
+  <si>
+    <t>1000 ETB</t>
+  </si>
+  <si>
+    <t>Nardos Hibist</t>
+  </si>
+  <si>
+    <t>1 Awash</t>
+  </si>
+  <si>
+    <t>Mulu Getaneh</t>
+  </si>
+  <si>
+    <t>30 Injera</t>
+  </si>
+  <si>
+    <t>Desybelew Amare</t>
+  </si>
+  <si>
+    <t>500 ETB and 1 Awash</t>
+  </si>
+  <si>
+    <t>Kelemie Amare</t>
+  </si>
+  <si>
+    <t>5000 ETB</t>
+  </si>
+  <si>
+    <t>Woyneshet</t>
+  </si>
+  <si>
+    <t>2 Pack of Water</t>
+  </si>
+  <si>
+    <t>Habtamu Mulu</t>
+  </si>
+  <si>
+    <t>Zelalem Mulu</t>
+  </si>
+  <si>
+    <t>2000 ETB</t>
+  </si>
+  <si>
+    <t>Bekalu Mulu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 Torta Cake and 2 Bottle of Awash </t>
+  </si>
+  <si>
+    <t>1 Box Beer and 1 Bottle of Guder</t>
+  </si>
+  <si>
+    <t>Beke</t>
+  </si>
+  <si>
+    <t>1 Black Label Whisky</t>
+  </si>
+  <si>
+    <t>Dilnesaw Mulu</t>
+  </si>
+  <si>
+    <t>0912730485</t>
+  </si>
+  <si>
+    <t>0915703961</t>
+  </si>
+  <si>
+    <t>0911261432</t>
+  </si>
+  <si>
+    <t>0923796372</t>
+  </si>
+  <si>
+    <t>0910928575</t>
+  </si>
+  <si>
+    <t>0913610789</t>
+  </si>
+  <si>
+    <t>0911131033</t>
+  </si>
+  <si>
+    <t>0948192027</t>
+  </si>
+  <si>
+    <t>0912650719</t>
+  </si>
+  <si>
+    <t>0984019201</t>
+  </si>
+  <si>
+    <t>0913979850</t>
+  </si>
+  <si>
+    <t>0911612976</t>
+  </si>
+  <si>
+    <t>0911439507</t>
+  </si>
+  <si>
+    <t>0911506655</t>
+  </si>
+  <si>
+    <t>0911500147</t>
+  </si>
+  <si>
+    <t>0944030979</t>
+  </si>
+  <si>
+    <t>0913024180</t>
   </si>
 </sst>
 </file>
@@ -92,8 +224,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -374,16 +507,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="1" max="1" width="21.28515625" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" customWidth="1"/>
+    <col min="3" max="3" width="31.42578125" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -399,49 +534,215 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2">
-        <v>912730485</v>
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3">
-        <v>922334455</v>
+        <v>5</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>39</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
-      <c r="B4">
-        <v>933445566</v>
+      <c r="B4" s="1" t="s">
+        <v>40</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
-      <c r="B5">
-        <v>944556677</v>
+      <c r="B5" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="C5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>9</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C16" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C17" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C18" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>37</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C20" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>